<commit_message>
funcionalidades para limpieza del dato a buscar
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Juan José\Documents\programas python\scraping_servientrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD01E693-82CB-4588-ABA9-71E2100E5959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62608BD8-DE8D-4D94-9E80-F970EECE3088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E416FBB-C6E1-4D3F-9E92-251C1E44CED1}"/>
   </bookViews>
@@ -34,34 +34,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>guia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2129030663          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2129017449          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2176030365          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2159984153          </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +78,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8734ED0-122E-4FC7-B0D4-4E2E0DB7EDB6}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -417,23 +414,348 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>231778496</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="1">
+        <v>2161788829</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="1">
+        <v>2162143803</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="1">
+        <v>2165877749</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>2167602235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>2169277038</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>9137160126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>9147007918</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>522760109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2095307865</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>2111368424</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>2111368431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>2123282428</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>2167602461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>2169146641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>2169933592</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2170422314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>9154439920</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>9155305065</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>2089161788</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>2089161812</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>2089161922</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>2089161941</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>2089166520</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>2092670202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>2104592813</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>2107373906</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>2107376639</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>2111374129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>2111381675</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>2111384338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>2111408816</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>2124902530</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>2131458302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>2131458587</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>2132213674</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>2132467190</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>2137035982</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>2143590008</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>2145353943</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>2154087258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>2154087259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>2159691695</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>2160511138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>2161855791</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>2170295802</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>2170295807</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>2170339631</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>2170506586</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>2170672262</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>2173706594</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>2174746520</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>3006323249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>3014462180</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>3041651686</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>3041652089</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>3041989991</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>3041991060</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>3044095813</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>3044139383</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>3044139471</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>3044415861</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>3044418127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>9147225713</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>9153467569</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>9154939023</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>9155305185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>9157577296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>9157957057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcciones error de carga de datos
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Juan José\Documents\programas python\scraping_servientrega\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62608BD8-DE8D-4D94-9E80-F970EECE3088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B57AD40-BA93-4433-B7ED-3F9CF32DF906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3E416FBB-C6E1-4D3F-9E92-251C1E44CED1}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:A70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -414,349 +414,244 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>231778496</v>
+      <c r="A2">
+        <v>2129031526</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>2161788829</v>
+      <c r="A3">
+        <v>2129034230</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2162143803</v>
+      <c r="A4">
+        <v>2129036584</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>2165877749</v>
+      <c r="A5">
+        <v>2139595988</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2167602235</v>
+      <c r="A6">
+        <v>2145085871</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>2169277038</v>
+      <c r="A7">
+        <v>2151145588</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>9137160126</v>
+      <c r="A8">
+        <v>2152483425</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>9147007918</v>
+      <c r="A9">
+        <v>2158670584</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>522760109</v>
+      <c r="A10">
+        <v>2164814489</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>2095307865</v>
+      <c r="A11">
+        <v>2167929154</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>2111368424</v>
+      <c r="A12">
+        <v>2167929401</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>2111368431</v>
+      <c r="A13">
+        <v>2171535321</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>2123282428</v>
+      <c r="A14">
+        <v>2171535509</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>2167602461</v>
+      <c r="A15">
+        <v>2171921928</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>2169146641</v>
+      <c r="A16">
+        <v>2173240654</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>2169933592</v>
+      <c r="A17">
+        <v>2173785485</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>2170422314</v>
+      <c r="A18">
+        <v>2176081466</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>9154439920</v>
+      <c r="A19">
+        <v>2176738241</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>9155305065</v>
+      <c r="A20">
+        <v>2176746209</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>2089161788</v>
+      <c r="A21">
+        <v>2176746924</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>2089161812</v>
+      <c r="A22">
+        <v>2176747539</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>2089161922</v>
+      <c r="A23">
+        <v>2176751705</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>2089161941</v>
+      <c r="A24">
+        <v>2176779765</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>2089166520</v>
+      <c r="A25">
+        <v>2176901371</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>2092670202</v>
+      <c r="A26">
+        <v>2176938657</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>2104592813</v>
+      <c r="A27">
+        <v>2176938663</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>2107373906</v>
+      <c r="A28">
+        <v>2179444401</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>2107376639</v>
+      <c r="A29">
+        <v>3011003965</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>2111374129</v>
+      <c r="A30">
+        <v>3014466745</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>2111381675</v>
+      <c r="A31">
+        <v>3020072394</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>2111384338</v>
+      <c r="A32">
+        <v>3041022504</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>2111408816</v>
+      <c r="A33">
+        <v>3043847040</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>2124902530</v>
+      <c r="A34">
+        <v>3045539096</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>2131458302</v>
+      <c r="A35">
+        <v>3047099382</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>2131458587</v>
+      <c r="A36">
+        <v>9156674647</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>2132213674</v>
+      <c r="A37">
+        <v>9159055187</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>2132467190</v>
+      <c r="A38">
+        <v>9159793527</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>2137035982</v>
+      <c r="A39">
+        <v>9159932900</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>2143590008</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>2145353943</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>2154087258</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>2154087259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>2159691695</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>2160511138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>2161855791</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>2170295802</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>2170295807</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>2170339631</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>2170506586</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>2170672262</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>2173706594</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>2174746520</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>3006323249</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>3014462180</v>
+      <c r="A40">
+        <v>9161309827</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>3041651686</v>
-      </c>
+      <c r="A56" s="1"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>3041652089</v>
-      </c>
+      <c r="A57" s="1"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>3041989991</v>
-      </c>
+      <c r="A58" s="1"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>3041991060</v>
-      </c>
+      <c r="A59" s="1"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>3044095813</v>
-      </c>
+      <c r="A60" s="1"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>3044139383</v>
-      </c>
+      <c r="A61" s="1"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>3044139471</v>
-      </c>
+      <c r="A62" s="1"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>3044415861</v>
-      </c>
+      <c r="A63" s="1"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>3044418127</v>
-      </c>
+      <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>9147225713</v>
-      </c>
+      <c r="A65" s="1"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>9153467569</v>
-      </c>
+      <c r="A66" s="1"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>9154939023</v>
-      </c>
+      <c r="A67" s="1"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
-        <v>9155305185</v>
-      </c>
+      <c r="A68" s="1"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>9157577296</v>
-      </c>
+      <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
-        <v>9157957057</v>
-      </c>
+      <c r="A70" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>